<commit_message>
Actualización automática 2025-06-03 09:15:07
</commit_message>
<xml_diff>
--- a/data/CHANDI ERAZO JOSUE.xlsx
+++ b/data/CHANDI ERAZO JOSUE.xlsx
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0</v>
+        <v>851.4299999999999</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>0</v>
@@ -818,7 +818,7 @@
       </c>
       <c r="K7" s="4" t="inlineStr">
         <is>
-          <t>0 de 5</t>
+          <t>1 de 5</t>
         </is>
       </c>
       <c r="L7" s="4" t="inlineStr">
@@ -861,7 +861,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -950,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>851.4299999999999</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -1048,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0</v>
+        <v>851.4299999999999</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización automática 2025-06-26 15:05:09
</commit_message>
<xml_diff>
--- a/data/CHANDI ERAZO JOSUE.xlsx
+++ b/data/CHANDI ERAZO JOSUE.xlsx
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0</v>
+        <v>157.15</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>0</v>
+        <v>2322.22</v>
       </c>
       <c r="R2" s="2" t="n">
         <v>0</v>
@@ -896,47 +896,47 @@
       </c>
       <c r="I7" s="4" t="inlineStr">
         <is>
+          <t>1 de 5</t>
+        </is>
+      </c>
+      <c r="J7" s="4" t="inlineStr">
+        <is>
           <t>0 de 5</t>
         </is>
       </c>
-      <c r="J7" s="4" t="inlineStr">
+      <c r="K7" s="4" t="inlineStr">
         <is>
           <t>0 de 5</t>
         </is>
       </c>
-      <c r="K7" s="4" t="inlineStr">
+      <c r="L7" s="4" t="inlineStr">
+        <is>
+          <t>1 de 5</t>
+        </is>
+      </c>
+      <c r="M7" s="4" t="inlineStr">
         <is>
           <t>0 de 5</t>
         </is>
       </c>
-      <c r="L7" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="O7" s="4" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="P7" s="4" t="inlineStr">
+        <is>
+          <t>0 de 5</t>
+        </is>
+      </c>
+      <c r="Q7" s="4" t="inlineStr">
         <is>
           <t>1 de 5</t>
-        </is>
-      </c>
-      <c r="M7" s="4" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
-        </is>
-      </c>
-      <c r="Q7" s="4" t="inlineStr">
-        <is>
-          <t>0 de 5</t>
         </is>
       </c>
       <c r="R7" s="4" t="inlineStr">
@@ -1031,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>-217.73</v>
+        <v>2261.64</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>0</v>
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>633.6999999999999</v>
+        <v>3113.07</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>0</v>
@@ -1356,13 +1356,13 @@
         <v>500</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>157.15</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>500</v>
+        <v>342.85</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>0.3143</v>
       </c>
     </row>
     <row r="8">
@@ -1500,13 +1500,13 @@
         <v>483</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0</v>
+        <v>2322.22</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>483</v>
+        <v>-1839.22</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0</v>
+        <v>4.807908902691511</v>
       </c>
     </row>
     <row r="14">
@@ -1591,13 +1591,13 @@
         <v>13500.0018254209</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>633.6999999999999</v>
+        <v>3113.07</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>12866.3018254209</v>
+        <v>10386.9318254209</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0.04694073439358535</v>
+        <v>0.2305977465971891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>